<commit_message>
Added coordinates of campus buildings
- createGraph.py now contains an array "coordinates" with the campus building coordinates
- nodeMap.png now shows the axis of the coordinate system with QNC as center
- DisMapCampus.xlsx now contains the coordinates as well
</commit_message>
<xml_diff>
--- a/Data/DistMapCampus.xlsx
+++ b/Data/DistMapCampus.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franz\OneDrive\Uni\Fall Term 2023\Co-op &amp; Adaptive Algorthms (ECE 457A)\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franz\Documents\GitHub\ece457_project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="19">
   <si>
     <t>CIF</t>
   </si>
@@ -69,6 +69,18 @@
   </si>
   <si>
     <t>V1</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>Distance between to buildings</t>
+  </si>
+  <si>
+    <t>Coordinates of a building</t>
   </si>
 </sst>
 </file>
@@ -92,7 +104,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -324,11 +336,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -347,6 +370,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -627,10 +652,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:T17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T18" sqref="T18"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -638,7 +663,7 @@
     <col min="1" max="16" width="4.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:20" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="8"/>
       <c r="B1" s="9" t="s">
         <v>0</v>
@@ -685,8 +710,15 @@
       <c r="P1" s="11" t="s">
         <v>13</v>
       </c>
+      <c r="R1" s="8"/>
+      <c r="S1" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="T1" s="11" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -735,8 +767,17 @@
       <c r="P2" s="12">
         <v>930</v>
       </c>
+      <c r="R2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="S2" s="6">
+        <v>-325</v>
+      </c>
+      <c r="T2" s="12">
+        <v>-515</v>
+      </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
@@ -785,8 +826,17 @@
       <c r="P3" s="13">
         <v>820</v>
       </c>
+      <c r="R3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="S3" s="2">
+        <v>-513</v>
+      </c>
+      <c r="T3" s="13">
+        <v>-55</v>
+      </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
@@ -835,8 +885,17 @@
       <c r="P4" s="13">
         <v>340</v>
       </c>
+      <c r="R4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="S4" s="2">
+        <v>738</v>
+      </c>
+      <c r="T4" s="13">
+        <v>115</v>
+      </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
@@ -885,8 +944,17 @@
       <c r="P5" s="13">
         <v>290</v>
       </c>
+      <c r="R5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="S5" s="2">
+        <v>50</v>
+      </c>
+      <c r="T5" s="13">
+        <v>156</v>
+      </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
@@ -935,8 +1003,17 @@
       <c r="P6" s="13">
         <v>440</v>
       </c>
+      <c r="R6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="S6" s="2">
+        <v>446</v>
+      </c>
+      <c r="T6" s="13">
+        <v>-244</v>
+      </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -985,8 +1062,17 @@
       <c r="P7" s="13">
         <v>440</v>
       </c>
+      <c r="R7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="S7" s="2">
+        <v>40</v>
+      </c>
+      <c r="T7" s="13">
+        <v>-123</v>
+      </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
@@ -1035,8 +1121,17 @@
       <c r="P8" s="13">
         <v>570</v>
       </c>
+      <c r="R8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="S8" s="2">
+        <v>-175</v>
+      </c>
+      <c r="T8" s="13">
+        <v>-111</v>
+      </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
@@ -1085,8 +1180,17 @@
       <c r="P9" s="13">
         <v>490</v>
       </c>
+      <c r="R9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="S9" s="2">
+        <v>-112</v>
+      </c>
+      <c r="T9" s="13">
+        <v>-78</v>
+      </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
@@ -1135,8 +1239,17 @@
       <c r="P10" s="13">
         <v>370</v>
       </c>
+      <c r="R10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="S10" s="2">
+        <v>0</v>
+      </c>
+      <c r="T10" s="13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
@@ -1185,8 +1298,17 @@
       <c r="P11" s="13">
         <v>170</v>
       </c>
+      <c r="R11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="S11" s="2">
+        <v>188</v>
+      </c>
+      <c r="T11" s="13">
+        <v>187</v>
+      </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A12" s="3" t="s">
         <v>9</v>
       </c>
@@ -1235,8 +1357,17 @@
       <c r="P12" s="13">
         <v>420</v>
       </c>
+      <c r="R12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="S12" s="2">
+        <v>227</v>
+      </c>
+      <c r="T12" s="13">
+        <v>-157</v>
+      </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
         <v>10</v>
       </c>
@@ -1285,8 +1416,17 @@
       <c r="P13" s="13">
         <v>270</v>
       </c>
+      <c r="R13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="S13" s="2">
+        <v>326</v>
+      </c>
+      <c r="T13" s="13">
+        <v>-55</v>
+      </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
         <v>11</v>
       </c>
@@ -1335,8 +1475,17 @@
       <c r="P14" s="13">
         <v>270</v>
       </c>
+      <c r="R14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="S14" s="2">
+        <v>65</v>
+      </c>
+      <c r="T14" s="13">
+        <v>382</v>
+      </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
         <v>12</v>
       </c>
@@ -1385,8 +1534,17 @@
       <c r="P15" s="13">
         <v>310</v>
       </c>
+      <c r="R15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="S15" s="2">
+        <v>78</v>
+      </c>
+      <c r="T15" s="13">
+        <v>82</v>
+      </c>
     </row>
-    <row r="16" spans="1:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:20" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A16" s="4" t="s">
         <v>13</v>
       </c>
@@ -1434,6 +1592,23 @@
       </c>
       <c r="P16" s="16">
         <v>0</v>
+      </c>
+      <c r="R16" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="S16" s="14">
+        <v>377</v>
+      </c>
+      <c r="T16" s="16">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A17" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="R17" s="19" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>